<commit_message>
Current dataset version of Status of
</commit_message>
<xml_diff>
--- a/assets/datasets/Estado_del_HPC_Colombia_Responses.xlsx
+++ b/assets/datasets/Estado_del_HPC_Colombia_Responses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ccb95d41fc86fae2/Documentos/cybercomputing/Articulos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eshernan/projects/cybercolombia.github.io/assets/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="11_430DC65513267F234A74611FF3D80653572BAF7B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60B6B573-80E5-C047-A3FB-C74DD3B48AE5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F5A63F7-2AA7-ED48-8C39-A01412EC1541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,13 +19,13 @@
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="208">
   <si>
     <t>Privada</t>
   </si>
@@ -1006,6 +1006,9 @@
   </si>
   <si>
     <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Con que tipo de instituciones colabora</t>
   </si>
 </sst>
 </file>
@@ -1336,7 +1339,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[Estado del HPC en Colombia  (Responses) - Form Responses 1.xlsx]Sheet1!PivotTable1</c:name>
+    <c:name>[Estado_del_HPC_Colombia_Responses.xlsx]Sheet1!PivotTable1</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -1437,36 +1440,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:marker>
-          <c:symbol val="diamond"/>
-          <c:size val="5"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent1">
-                    <a:tint val="100000"/>
-                    <a:shade val="100000"/>
-                    <a:satMod val="129999"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent1">
-                    <a:tint val="50000"/>
-                    <a:shade val="100000"/>
-                    <a:satMod val="350000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="16200000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -2435,10 +2409,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Esteban Hernandez" refreshedDate="45851.971112384257" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="10" xr:uid="{EADAFD08-C127-2143-A440-03A43BF8B770}">
   <cacheSource type="worksheet">
@@ -2821,7 +2791,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A64AD267-8ED9-DC40-8913-414F0D09DF1B}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A64AD267-8ED9-DC40-8913-414F0D09DF1B}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="5">
   <location ref="C4:D7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="26">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -3957,8 +3927,8 @@
   <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="Z1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB1" sqref="AB1"/>
+      <pane xSplit="1" topLeftCell="O1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4036,7 +4006,7 @@
         <v>14</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>15</v>
+        <v>207</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>16</v>

</xml_diff>